<commit_message>
Parameterized Tests with Exel Files
</commit_message>
<xml_diff>
--- a/src/test/resources/BookItQa3.xlsx
+++ b/src/test/resources/BookItQa3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamaldemir/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\IdeaProjects\AllEnvironmentVerification_EU8\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C3FA22-B865-DB4E-83FB-41BEAEC8C5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6519D08A-523D-4B5B-BB16-57B0965B33B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="2660" windowWidth="28040" windowHeight="17440" xr2:uid="{EE4F955A-F690-2F49-9A0F-2DC077CE6888}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EE4F955A-F690-2F49-9A0F-2DC077CE6888}"/>
   </bookViews>
   <sheets>
     <sheet name="QA3" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,37 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="556">
-  <si>
-    <t>admin@mail.com</t>
-  </si>
-  <si>
-    <t>nedstark</t>
-  </si>
-  <si>
-    <t>jalabaster7f@drupal.org</t>
-  </si>
-  <si>
-    <t>terimapam</t>
-  </si>
-  <si>
-    <t>sdarben7g@alibaba.com</t>
-  </si>
-  <si>
-    <t>angiecoatham</t>
-  </si>
-  <si>
-    <t>aneagle7h@miibeian.gov.cn</t>
-  </si>
-  <si>
-    <t>bennetttomanek</t>
-  </si>
-  <si>
-    <t>ewrist7i@livejournal.com</t>
-  </si>
-  <si>
-    <t>marianndewi</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="546">
   <si>
     <t>gmalkin7j@mail.ru</t>
   </si>
@@ -2053,27 +2021,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91BD84C-CFFD-594B-8C7D-0C30CE6C2E0C}">
-  <dimension ref="A1:B281"/>
+  <dimension ref="A1:B276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="B1" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2081,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2089,7 +2057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2105,7 +2073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2113,7 +2081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2121,7 +2089,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2129,7 +2097,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2137,7 +2105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2145,7 +2113,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2153,7 +2121,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2161,7 +2129,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2169,7 +2137,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2177,7 +2145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2185,7 +2153,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2193,7 +2161,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2201,7 +2169,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2209,7 +2177,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2217,7 +2185,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2225,7 +2193,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2233,7 +2201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2241,7 +2209,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2249,7 +2217,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2257,7 +2225,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2265,7 +2233,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2273,7 +2241,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2281,7 +2249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2289,7 +2257,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2297,7 +2265,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2305,7 +2273,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2313,7 +2281,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -2321,7 +2289,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -2329,7 +2297,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2337,7 +2305,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -2345,7 +2313,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2353,7 +2321,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -2361,7 +2329,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2369,7 +2337,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -2377,7 +2345,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -2385,7 +2353,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -2393,7 +2361,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -2401,7 +2369,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -2409,7 +2377,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2417,7 +2385,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -2425,7 +2393,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2433,7 +2401,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2441,7 +2409,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2449,7 +2417,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -2457,7 +2425,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -2465,7 +2433,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -2473,7 +2441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -2481,7 +2449,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -2489,7 +2457,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -2497,7 +2465,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -2505,7 +2473,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -2513,7 +2481,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -2521,7 +2489,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -2529,7 +2497,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -2537,7 +2505,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -2545,7 +2513,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -2553,7 +2521,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -2561,7 +2529,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -2569,7 +2537,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -2577,7 +2545,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>126</v>
       </c>
@@ -2585,7 +2553,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>128</v>
       </c>
@@ -2593,7 +2561,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -2601,7 +2569,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -2609,7 +2577,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -2617,7 +2585,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -2625,7 +2593,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -2633,7 +2601,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -2641,7 +2609,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -2649,7 +2617,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -2657,7 +2625,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -2665,7 +2633,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -2673,7 +2641,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -2681,7 +2649,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -2689,7 +2657,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>154</v>
       </c>
@@ -2697,7 +2665,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>156</v>
       </c>
@@ -2705,7 +2673,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -2713,7 +2681,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -2721,7 +2689,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -2729,7 +2697,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -2737,7 +2705,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>166</v>
       </c>
@@ -2745,7 +2713,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -2753,7 +2721,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>170</v>
       </c>
@@ -2761,7 +2729,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -2769,7 +2737,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -2777,7 +2745,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>176</v>
       </c>
@@ -2785,7 +2753,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -2793,7 +2761,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -2801,7 +2769,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -2809,7 +2777,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -2817,7 +2785,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -2825,7 +2793,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -2833,7 +2801,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -2841,7 +2809,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>192</v>
       </c>
@@ -2849,7 +2817,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>194</v>
       </c>
@@ -2857,7 +2825,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>196</v>
       </c>
@@ -2865,7 +2833,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>198</v>
       </c>
@@ -2873,7 +2841,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>200</v>
       </c>
@@ -2881,7 +2849,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>202</v>
       </c>
@@ -2889,7 +2857,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>204</v>
       </c>
@@ -2897,7 +2865,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>206</v>
       </c>
@@ -2905,7 +2873,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>208</v>
       </c>
@@ -2913,7 +2881,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>210</v>
       </c>
@@ -2921,7 +2889,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>212</v>
       </c>
@@ -2929,7 +2897,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>214</v>
       </c>
@@ -2937,7 +2905,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>216</v>
       </c>
@@ -2945,7 +2913,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>218</v>
       </c>
@@ -2953,7 +2921,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>220</v>
       </c>
@@ -2961,7 +2929,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>222</v>
       </c>
@@ -2969,7 +2937,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>224</v>
       </c>
@@ -2977,7 +2945,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>226</v>
       </c>
@@ -2985,7 +2953,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>228</v>
       </c>
@@ -2993,7 +2961,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>230</v>
       </c>
@@ -3001,7 +2969,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>232</v>
       </c>
@@ -3009,7 +2977,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>234</v>
       </c>
@@ -3017,7 +2985,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>236</v>
       </c>
@@ -3025,7 +2993,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>238</v>
       </c>
@@ -3033,7 +3001,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>240</v>
       </c>
@@ -3041,7 +3009,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>242</v>
       </c>
@@ -3049,7 +3017,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>244</v>
       </c>
@@ -3057,7 +3025,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>246</v>
       </c>
@@ -3065,7 +3033,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>248</v>
       </c>
@@ -3073,7 +3041,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>250</v>
       </c>
@@ -3081,7 +3049,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>252</v>
       </c>
@@ -3089,7 +3057,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>254</v>
       </c>
@@ -3097,7 +3065,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>256</v>
       </c>
@@ -3105,7 +3073,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>258</v>
       </c>
@@ -3113,7 +3081,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>260</v>
       </c>
@@ -3121,7 +3089,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>262</v>
       </c>
@@ -3129,7 +3097,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>264</v>
       </c>
@@ -3137,7 +3105,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>266</v>
       </c>
@@ -3145,7 +3113,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>268</v>
       </c>
@@ -3153,7 +3121,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>270</v>
       </c>
@@ -3161,7 +3129,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>272</v>
       </c>
@@ -3169,7 +3137,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>274</v>
       </c>
@@ -3177,7 +3145,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>276</v>
       </c>
@@ -3185,7 +3153,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>278</v>
       </c>
@@ -3193,7 +3161,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>280</v>
       </c>
@@ -3201,7 +3169,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>282</v>
       </c>
@@ -3209,7 +3177,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>284</v>
       </c>
@@ -3217,7 +3185,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>286</v>
       </c>
@@ -3225,7 +3193,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>288</v>
       </c>
@@ -3233,7 +3201,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>290</v>
       </c>
@@ -3241,7 +3209,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>292</v>
       </c>
@@ -3249,7 +3217,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>294</v>
       </c>
@@ -3257,7 +3225,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>296</v>
       </c>
@@ -3265,7 +3233,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>298</v>
       </c>
@@ -3273,7 +3241,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>300</v>
       </c>
@@ -3281,7 +3249,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>302</v>
       </c>
@@ -3289,7 +3257,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>304</v>
       </c>
@@ -3297,7 +3265,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>306</v>
       </c>
@@ -3305,7 +3273,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>308</v>
       </c>
@@ -3313,7 +3281,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>310</v>
       </c>
@@ -3321,7 +3289,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>312</v>
       </c>
@@ -3329,7 +3297,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>314</v>
       </c>
@@ -3337,7 +3305,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>316</v>
       </c>
@@ -3345,7 +3313,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>318</v>
       </c>
@@ -3353,7 +3321,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>320</v>
       </c>
@@ -3361,7 +3329,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>322</v>
       </c>
@@ -3369,7 +3337,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>324</v>
       </c>
@@ -3377,7 +3345,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>326</v>
       </c>
@@ -3385,7 +3353,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>328</v>
       </c>
@@ -3393,7 +3361,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>330</v>
       </c>
@@ -3401,7 +3369,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>332</v>
       </c>
@@ -3409,7 +3377,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>334</v>
       </c>
@@ -3417,7 +3385,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>336</v>
       </c>
@@ -3425,7 +3393,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>338</v>
       </c>
@@ -3433,7 +3401,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>340</v>
       </c>
@@ -3441,7 +3409,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>342</v>
       </c>
@@ -3449,7 +3417,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>344</v>
       </c>
@@ -3457,7 +3425,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>346</v>
       </c>
@@ -3465,7 +3433,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>348</v>
       </c>
@@ -3473,7 +3441,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>350</v>
       </c>
@@ -3481,7 +3449,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>352</v>
       </c>
@@ -3489,7 +3457,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>354</v>
       </c>
@@ -3497,7 +3465,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -3505,7 +3473,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>358</v>
       </c>
@@ -3513,7 +3481,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>360</v>
       </c>
@@ -3521,7 +3489,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>362</v>
       </c>
@@ -3529,7 +3497,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>364</v>
       </c>
@@ -3537,7 +3505,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>366</v>
       </c>
@@ -3545,7 +3513,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>368</v>
       </c>
@@ -3553,7 +3521,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>370</v>
       </c>
@@ -3561,7 +3529,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>372</v>
       </c>
@@ -3569,7 +3537,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>374</v>
       </c>
@@ -3577,7 +3545,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>376</v>
       </c>
@@ -3585,7 +3553,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>378</v>
       </c>
@@ -3593,7 +3561,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>380</v>
       </c>
@@ -3601,7 +3569,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>382</v>
       </c>
@@ -3609,7 +3577,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>384</v>
       </c>
@@ -3617,7 +3585,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>386</v>
       </c>
@@ -3625,7 +3593,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>388</v>
       </c>
@@ -3633,7 +3601,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>390</v>
       </c>
@@ -3641,7 +3609,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>392</v>
       </c>
@@ -3649,7 +3617,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>394</v>
       </c>
@@ -3657,7 +3625,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>396</v>
       </c>
@@ -3665,7 +3633,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>398</v>
       </c>
@@ -3673,7 +3641,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>400</v>
       </c>
@@ -3681,7 +3649,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>402</v>
       </c>
@@ -3689,7 +3657,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>404</v>
       </c>
@@ -3697,7 +3665,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>406</v>
       </c>
@@ -3705,7 +3673,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>408</v>
       </c>
@@ -3713,7 +3681,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>410</v>
       </c>
@@ -3721,7 +3689,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>412</v>
       </c>
@@ -3729,7 +3697,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>414</v>
       </c>
@@ -3737,7 +3705,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>416</v>
       </c>
@@ -3745,7 +3713,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>418</v>
       </c>
@@ -3753,7 +3721,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>420</v>
       </c>
@@ -3761,7 +3729,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>422</v>
       </c>
@@ -3769,7 +3737,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>424</v>
       </c>
@@ -3777,7 +3745,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>426</v>
       </c>
@@ -3785,7 +3753,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>428</v>
       </c>
@@ -3793,7 +3761,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>430</v>
       </c>
@@ -3801,7 +3769,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>432</v>
       </c>
@@ -3809,7 +3777,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>434</v>
       </c>
@@ -3817,7 +3785,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>436</v>
       </c>
@@ -3825,7 +3793,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>438</v>
       </c>
@@ -3833,7 +3801,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>440</v>
       </c>
@@ -3841,7 +3809,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>442</v>
       </c>
@@ -3849,7 +3817,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>444</v>
       </c>
@@ -3857,7 +3825,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>446</v>
       </c>
@@ -3865,7 +3833,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>448</v>
       </c>
@@ -3873,7 +3841,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>450</v>
       </c>
@@ -3881,7 +3849,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>452</v>
       </c>
@@ -3889,7 +3857,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>454</v>
       </c>
@@ -3897,7 +3865,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>456</v>
       </c>
@@ -3905,7 +3873,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>458</v>
       </c>
@@ -3913,7 +3881,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>460</v>
       </c>
@@ -3921,7 +3889,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>462</v>
       </c>
@@ -3929,7 +3897,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>464</v>
       </c>
@@ -3937,7 +3905,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>466</v>
       </c>
@@ -3945,7 +3913,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>468</v>
       </c>
@@ -3953,7 +3921,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>470</v>
       </c>
@@ -3961,7 +3929,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>472</v>
       </c>
@@ -3969,7 +3937,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>474</v>
       </c>
@@ -3977,7 +3945,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>476</v>
       </c>
@@ -3985,7 +3953,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>478</v>
       </c>
@@ -3993,7 +3961,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>480</v>
       </c>
@@ -4001,7 +3969,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>482</v>
       </c>
@@ -4009,7 +3977,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>484</v>
       </c>
@@ -4017,7 +3985,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>486</v>
       </c>
@@ -4025,7 +3993,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>488</v>
       </c>
@@ -4033,7 +4001,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>490</v>
       </c>
@@ -4041,7 +4009,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>492</v>
       </c>
@@ -4049,7 +4017,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>494</v>
       </c>
@@ -4057,7 +4025,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>496</v>
       </c>
@@ -4065,7 +4033,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>498</v>
       </c>
@@ -4073,7 +4041,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>500</v>
       </c>
@@ -4081,7 +4049,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>502</v>
       </c>
@@ -4089,7 +4057,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>504</v>
       </c>
@@ -4097,7 +4065,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>506</v>
       </c>
@@ -4105,7 +4073,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>508</v>
       </c>
@@ -4113,79 +4081,79 @@
         <v>509</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>510</v>
       </c>
       <c r="B257" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A258" t="s">
+      <c r="B258" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
         <v>512</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B259" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A259" t="s">
+      <c r="B260" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
         <v>514</v>
       </c>
-      <c r="B259" t="s">
+      <c r="B261" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A260" t="s">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
         <v>516</v>
       </c>
-      <c r="B260" t="s">
+      <c r="B262" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A261" t="s">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
         <v>518</v>
-      </c>
-      <c r="B261" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A262" t="s">
-        <v>520</v>
-      </c>
-      <c r="B262" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A263" t="s">
-        <v>521</v>
       </c>
       <c r="B263" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
+        <v>520</v>
+      </c>
+      <c r="B264" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
         <v>522</v>
       </c>
-      <c r="B264" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A265" t="s">
+      <c r="B265" t="s">
         <v>523</v>
       </c>
-      <c r="B265" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>524</v>
       </c>
@@ -4193,7 +4161,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>526</v>
       </c>
@@ -4201,7 +4169,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>528</v>
       </c>
@@ -4209,7 +4177,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>530</v>
       </c>
@@ -4217,7 +4185,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>532</v>
       </c>
@@ -4225,92 +4193,52 @@
         <v>533</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>534</v>
       </c>
       <c r="B271" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A272" t="s">
+      <c r="B272" t="s">
         <v>536</v>
       </c>
-      <c r="B272" t="s">
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A273" t="s">
+      <c r="B273" t="s">
         <v>538</v>
       </c>
-      <c r="B273" t="s">
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A274" t="s">
+      <c r="B274" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
         <v>540</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B275" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" t="s">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
         <v>542</v>
-      </c>
-      <c r="B275" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" t="s">
-        <v>544</v>
       </c>
       <c r="B276" t="s">
         <v>543</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" t="s">
-        <v>545</v>
-      </c>
-      <c r="B277" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A278" t="s">
-        <v>547</v>
-      </c>
-      <c r="B278" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A279" t="s">
-        <v>549</v>
-      </c>
-      <c r="B279" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" t="s">
-        <v>550</v>
-      </c>
-      <c r="B280" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A281" t="s">
-        <v>552</v>
-      </c>
-      <c r="B281" t="s">
-        <v>553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>